<commit_message>
feat: non-linear lift calculation using decambering method
</commit_message>
<xml_diff>
--- a/Airfoil_Data/Airfoil Data.xlsx
+++ b/Airfoil_Data/Airfoil Data.xlsx
@@ -16,9 +16,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="5">
   <si>
-    <t>AOA_Zero</t>
+    <t>AOA_zero</t>
   </si>
   <si>
     <t>Reynolds</t>
@@ -26,12 +26,18 @@
   <si>
     <t xml:space="preserve">CL_max </t>
   </si>
+  <si>
+    <t>AOA_exp</t>
+  </si>
+  <si>
+    <t>CL_exp</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -46,6 +52,10 @@
     <font>
       <color theme="1"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Menlo"/>
     </font>
   </fonts>
   <fills count="2">
@@ -62,7 +72,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -73,6 +83,12 @@
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="11" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="11" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -321,6 +337,12 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2">
@@ -332,6 +354,12 @@
       <c r="C2" s="1">
         <v>1.51</v>
       </c>
+      <c r="D2" s="4">
+        <v>-17.1694</v>
+      </c>
+      <c r="E2" s="4">
+        <v>-1.2608</v>
+      </c>
     </row>
     <row r="3">
       <c r="B3" s="3">
@@ -340,13 +368,481 @@
       <c r="C3" s="1">
         <v>1.55</v>
       </c>
+      <c r="D3" s="4">
+        <v>-15.9293</v>
+      </c>
+      <c r="E3" s="4">
+        <v>-1.3424</v>
+      </c>
     </row>
     <row r="4">
       <c r="B4" s="3">
-        <v>8800000.0</v>
+        <v>9000000.0</v>
       </c>
       <c r="C4" s="1">
         <v>1.6123</v>
+      </c>
+      <c r="D4" s="4">
+        <v>-16.0592</v>
+      </c>
+      <c r="E4" s="4">
+        <v>-1.4651</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="D5" s="4">
+        <v>-15.7798</v>
+      </c>
+      <c r="E5" s="4">
+        <v>-1.5469</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="D6" s="4">
+        <v>-15.2328</v>
+      </c>
+      <c r="E6" s="4">
+        <v>-1.5127</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="D7" s="4">
+        <v>-14.2761</v>
+      </c>
+      <c r="E7" s="4">
+        <v>-1.4444</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="D8" s="4">
+        <v>-13.1826</v>
+      </c>
+      <c r="E8" s="4">
+        <v>-1.3694</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="D9" s="4">
+        <v>-11.9534</v>
+      </c>
+      <c r="E9" s="4">
+        <v>-1.267</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="D10" s="4">
+        <v>-11.1351</v>
+      </c>
+      <c r="E10" s="4">
+        <v>-1.1783</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="D11" s="4">
+        <v>-10.3165</v>
+      </c>
+      <c r="E11" s="4">
+        <v>-1.0964</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="D12" s="4">
+        <v>-9.2262</v>
+      </c>
+      <c r="E12" s="4">
+        <v>-0.9668</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="D13" s="4">
+        <v>-8.2711</v>
+      </c>
+      <c r="E13" s="4">
+        <v>-0.8713</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="D14" s="4">
+        <v>-7.5897</v>
+      </c>
+      <c r="E14" s="4">
+        <v>-0.7894</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="D15" s="4">
+        <v>-7.0448</v>
+      </c>
+      <c r="E15" s="4">
+        <v>-0.7212</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="D16" s="4">
+        <v>-6.4986</v>
+      </c>
+      <c r="E16" s="4">
+        <v>-0.6734</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="D17" s="4">
+        <v>-5.8164</v>
+      </c>
+      <c r="E17" s="4">
+        <v>-0.6052</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="D18" s="4">
+        <v>-5.2702</v>
+      </c>
+      <c r="E18" s="4">
+        <v>-0.5574</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="D19" s="4">
+        <v>-4.7253</v>
+      </c>
+      <c r="E19" s="4">
+        <v>-0.4892</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="D20" s="4">
+        <v>-4.0427</v>
+      </c>
+      <c r="E20" s="4">
+        <v>-0.4278</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="D21" s="4">
+        <v>-3.3605</v>
+      </c>
+      <c r="E21" s="4">
+        <v>-0.3596</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="D22" s="4">
+        <v>-3.0896</v>
+      </c>
+      <c r="E22" s="4">
+        <v>-0.2982</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="D23" s="4">
+        <v>-2.4062</v>
+      </c>
+      <c r="E23" s="4">
+        <v>-0.2504</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="D24" s="4">
+        <v>-1.9965</v>
+      </c>
+      <c r="E24" s="4">
+        <v>-0.2163</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="D25" s="4">
+        <v>-1.3147</v>
+      </c>
+      <c r="E25" s="4">
+        <v>-0.1412</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="D26" s="4">
+        <v>-0.7693</v>
+      </c>
+      <c r="E26" s="4">
+        <v>-0.0798</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="D27" s="4">
+        <v>-0.3604</v>
+      </c>
+      <c r="E27" s="4">
+        <v>-0.0321</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="D28" s="4">
+        <v>0.1862</v>
+      </c>
+      <c r="E28" s="4">
+        <v>0.0089</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="D29" s="4">
+        <v>0.4574</v>
+      </c>
+      <c r="E29" s="4">
+        <v>0.0634</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="D30" s="4">
+        <v>0.8667</v>
+      </c>
+      <c r="E30" s="4">
+        <v>0.1044</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="D31" s="4">
+        <v>1.2757</v>
+      </c>
+      <c r="E31" s="4">
+        <v>0.1521</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="D32" s="4">
+        <v>1.685</v>
+      </c>
+      <c r="E32" s="4">
+        <v>0.1931</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="D33" s="4">
+        <v>2.0943</v>
+      </c>
+      <c r="E33" s="4">
+        <v>0.234</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="D34" s="4">
+        <v>2.5036</v>
+      </c>
+      <c r="E34" s="4">
+        <v>0.2749</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="D35" s="4">
+        <v>2.7753</v>
+      </c>
+      <c r="E35" s="4">
+        <v>0.3227</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="D36" s="4">
+        <v>3.3223</v>
+      </c>
+      <c r="E36" s="4">
+        <v>0.3568</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="D37" s="4">
+        <v>4.0033</v>
+      </c>
+      <c r="E37" s="4">
+        <v>0.4455</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="D38" s="4">
+        <v>5.2316</v>
+      </c>
+      <c r="E38" s="4">
+        <v>0.5615</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="D39" s="4">
+        <v>6.1871</v>
+      </c>
+      <c r="E39" s="4">
+        <v>0.6502</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="D40" s="4">
+        <v>6.8665</v>
+      </c>
+      <c r="E40" s="4">
+        <v>0.7661</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="D41" s="4">
+        <v>7.5483</v>
+      </c>
+      <c r="E41" s="4">
+        <v>0.8412</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="D42" s="4">
+        <v>8.2297</v>
+      </c>
+      <c r="E42" s="4">
+        <v>0.923</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="D43" s="4">
+        <v>8.9119</v>
+      </c>
+      <c r="E43" s="4">
+        <v>0.9913</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="D44" s="4">
+        <v>9.5941</v>
+      </c>
+      <c r="E44" s="4">
+        <v>1.0595</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="D45" s="4">
+        <v>10.2767</v>
+      </c>
+      <c r="E45" s="4">
+        <v>1.1209</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="D46" s="4">
+        <v>10.8216</v>
+      </c>
+      <c r="E46" s="4">
+        <v>1.1891</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="D47" s="4">
+        <v>11.2313</v>
+      </c>
+      <c r="E47" s="4">
+        <v>1.2233</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="D48" s="4">
+        <v>12.1893</v>
+      </c>
+      <c r="E48" s="4">
+        <v>1.2711</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="D49" s="4">
+        <v>13.2812</v>
+      </c>
+      <c r="E49" s="4">
+        <v>1.3734</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="D50" s="4">
+        <v>14.2375</v>
+      </c>
+      <c r="E50" s="4">
+        <v>1.4485</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="D51" s="4">
+        <v>15.1946</v>
+      </c>
+      <c r="E51" s="4">
+        <v>1.51</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="D52" s="4">
+        <v>16.4238</v>
+      </c>
+      <c r="E52" s="4">
+        <v>1.6123</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="D53" s="4">
+        <v>16.4291</v>
+      </c>
+      <c r="E53" s="4">
+        <v>1.5237</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="D54" s="4">
+        <v>16.5725</v>
+      </c>
+      <c r="E54" s="4">
+        <v>1.4215</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="D55" s="4">
+        <v>16.9883</v>
+      </c>
+      <c r="E55" s="4">
+        <v>1.3534</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="D56" s="4">
+        <v>17.4074</v>
+      </c>
+      <c r="E56" s="4">
+        <v>1.2308</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="D57" s="4">
+        <v>17.5532</v>
+      </c>
+      <c r="E57" s="4">
+        <v>1.0877</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="D58" s="4">
+        <v>18.1095</v>
+      </c>
+      <c r="E58" s="4">
+        <v>0.9651</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="D59" s="4">
+        <v>19.348</v>
+      </c>
+      <c r="E59" s="4">
+        <v>0.9108</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="D60" s="4">
+        <v>20.174</v>
+      </c>
+      <c r="E60" s="4">
+        <v>0.87</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="D61" s="4">
+        <v>21.0</v>
+      </c>
+      <c r="E61" s="4">
+        <v>0.87</v>
       </c>
     </row>
   </sheetData>
@@ -374,6 +870,12 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1">
@@ -385,6 +887,12 @@
       <c r="C2" s="1">
         <v>1.6284</v>
       </c>
+      <c r="D2" s="4">
+        <v>-10.15355844</v>
+      </c>
+      <c r="E2" s="4">
+        <v>-0.920103896</v>
+      </c>
     </row>
     <row r="3">
       <c r="B3" s="3">
@@ -393,7 +901,12 @@
       <c r="C3" s="1">
         <v>1.7794</v>
       </c>
-      <c r="D3" s="3"/>
+      <c r="D3" s="5">
+        <v>-8.233558442</v>
+      </c>
+      <c r="E3" s="4">
+        <v>-0.713437229</v>
+      </c>
     </row>
     <row r="4">
       <c r="B4" s="3">
@@ -401,6 +914,148 @@
       </c>
       <c r="C4" s="1">
         <v>1.8172</v>
+      </c>
+      <c r="D4" s="4">
+        <v>-5.129974026</v>
+      </c>
+      <c r="E4" s="4">
+        <v>-0.388606061</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="D5" s="4">
+        <v>-2.473558442</v>
+      </c>
+      <c r="E5" s="4">
+        <v>-0.093437229</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="D6" s="4">
+        <v>-0.257662338</v>
+      </c>
+      <c r="E6" s="4">
+        <v>0.142770563</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="D7" s="4">
+        <v>1.808623377</v>
+      </c>
+      <c r="E7" s="4">
+        <v>0.371532468</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="D8" s="4">
+        <v>3.881558442</v>
+      </c>
+      <c r="E8" s="4">
+        <v>0.570995671</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="D9" s="4">
+        <v>5.801558442</v>
+      </c>
+      <c r="E9" s="4">
+        <v>0.777662338</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="D10" s="4">
+        <v>8.017454545</v>
+      </c>
+      <c r="E10" s="4">
+        <v>1.01387013</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="D11" s="4">
+        <v>9.942441558</v>
+      </c>
+      <c r="E11" s="4">
+        <v>1.198562771</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="D12" s="4">
+        <v>11.85745455</v>
+      </c>
+      <c r="E12" s="4">
+        <v>1.427203463</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="D13" s="4">
+        <v>13.93537662</v>
+      </c>
+      <c r="E13" s="4">
+        <v>1.604692641</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="D14" s="4">
+        <v>16.02327273</v>
+      </c>
+      <c r="E14" s="4">
+        <v>1.738233766</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="D15" s="4">
+        <v>16.768</v>
+      </c>
+      <c r="E15" s="4">
+        <v>1.790112554</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="D16" s="4">
+        <v>17.52103896</v>
+      </c>
+      <c r="E16" s="4">
+        <v>1.805367965</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="D17" s="4">
+        <v>17.97319481</v>
+      </c>
+      <c r="E17" s="4">
+        <v>1.8172</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="D18" s="4">
+        <v>18.432</v>
+      </c>
+      <c r="E18" s="4">
+        <v>1.791445887</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="D19" s="4">
+        <v>18.62815584</v>
+      </c>
+      <c r="E19" s="4">
+        <v>1.593800866</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="D20" s="4">
+        <v>19.06202597</v>
+      </c>
+      <c r="E20" s="4">
+        <v>1.015393939</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="D21" s="4">
+        <v>20.13257143</v>
+      </c>
+      <c r="E21" s="4">
+        <v>0.964969697</v>
       </c>
     </row>
   </sheetData>
@@ -428,6 +1083,12 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1">
@@ -439,6 +1100,12 @@
       <c r="C2" s="1">
         <v>1.4434</v>
       </c>
+      <c r="D2" s="4">
+        <v>-12.17560976</v>
+      </c>
+      <c r="E2" s="4">
+        <v>-0.827</v>
+      </c>
     </row>
     <row r="3">
       <c r="B3" s="3">
@@ -447,13 +1114,145 @@
       <c r="C3" s="1">
         <v>1.5144</v>
       </c>
+      <c r="D3" s="4">
+        <v>-10.30243902</v>
+      </c>
+      <c r="E3" s="4">
+        <v>-0.661</v>
+      </c>
     </row>
     <row r="4">
       <c r="B4" s="3">
-        <v>8800000.0</v>
+        <v>9000000.0</v>
       </c>
       <c r="C4" s="1">
         <v>1.546</v>
+      </c>
+      <c r="D4" s="4">
+        <v>-8.429268293</v>
+      </c>
+      <c r="E4" s="4">
+        <v>-0.495</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="D5" s="4">
+        <v>-5.931707317</v>
+      </c>
+      <c r="E5" s="4">
+        <v>-0.203</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="D6" s="4">
+        <v>-3.746341463</v>
+      </c>
+      <c r="E6" s="4">
+        <v>0.019</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="D7" s="4">
+        <v>-1.873170732</v>
+      </c>
+      <c r="E7" s="4">
+        <v>0.232</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="D8" s="4">
+        <v>0.312195122</v>
+      </c>
+      <c r="E8" s="4">
+        <v>0.422</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="D9" s="4">
+        <v>2.185365854</v>
+      </c>
+      <c r="E9" s="4">
+        <v>0.628</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="D10" s="4">
+        <v>4.214634146</v>
+      </c>
+      <c r="E10" s="4">
+        <v>0.81</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="D11" s="4">
+        <v>6.087804878</v>
+      </c>
+      <c r="E11" s="4">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="D12" s="4">
+        <v>8.117073171</v>
+      </c>
+      <c r="E12" s="4">
+        <v>1.182</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="D13" s="4">
+        <v>10.45853659</v>
+      </c>
+      <c r="E13" s="4">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="D14" s="4">
+        <v>12.33170732</v>
+      </c>
+      <c r="E14" s="4">
+        <v>1.403</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="D15" s="4">
+        <v>14.36097561</v>
+      </c>
+      <c r="E15" s="4">
+        <v>1.443</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="D16" s="4">
+        <v>16.3902439</v>
+      </c>
+      <c r="E16" s="4">
+        <v>1.404</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="D17" s="4">
+        <v>18.4195122</v>
+      </c>
+      <c r="E17" s="4">
+        <v>1.31</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="D18" s="4">
+        <v>22.0</v>
+      </c>
+      <c r="E18" s="4">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="D19" s="4">
+        <v>23.0</v>
+      </c>
+      <c r="E19" s="4">
+        <v>0.8</v>
       </c>
     </row>
   </sheetData>
@@ -481,6 +1280,12 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1">
@@ -492,6 +1297,12 @@
       <c r="C2" s="1">
         <v>1.7344</v>
       </c>
+      <c r="D2" s="4">
+        <v>-4.2</v>
+      </c>
+      <c r="E2" s="4">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="3">
       <c r="B3" s="3">
@@ -500,13 +1311,449 @@
       <c r="C3" s="1">
         <v>1.8013</v>
       </c>
+      <c r="D3" s="4">
+        <v>-0.072260824</v>
+      </c>
+      <c r="E3" s="4">
+        <v>0.425165563</v>
+      </c>
     </row>
     <row r="4">
       <c r="B4" s="3">
-        <v>8800000.0</v>
+        <v>1.0E7</v>
       </c>
       <c r="C4" s="1">
         <v>1.819</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0.68887956</v>
+      </c>
+      <c r="E4" s="4">
+        <v>0.506622517</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="D5" s="4">
+        <v>1.925458574</v>
+      </c>
+      <c r="E5" s="4">
+        <v>0.633774834</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="D6" s="4">
+        <v>2.687016651</v>
+      </c>
+      <c r="E6" s="4">
+        <v>0.723178808</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="D7" s="4">
+        <v>3.637998333</v>
+      </c>
+      <c r="E7" s="4">
+        <v>0.816556291</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="D8" s="4">
+        <v>4.779239006</v>
+      </c>
+      <c r="E8" s="4">
+        <v>0.929801325</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="D9" s="4">
+        <v>5.82524576</v>
+      </c>
+      <c r="E9" s="4">
+        <v>1.031125828</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="D10" s="4">
+        <v>6.776645135</v>
+      </c>
+      <c r="E10" s="4">
+        <v>1.132450331</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="D11" s="4">
+        <v>7.727626817</v>
+      </c>
+      <c r="E11" s="4">
+        <v>1.225827815</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="D12" s="4">
+        <v>8.773320301</v>
+      </c>
+      <c r="E12" s="4">
+        <v>1.321192053</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="D13" s="4">
+        <v>9.723779868</v>
+      </c>
+      <c r="E13" s="4">
+        <v>1.404635762</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="D14" s="4">
+        <v>10.76905566</v>
+      </c>
+      <c r="E14" s="4">
+        <v>1.49205298</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="D15" s="4">
+        <v>11.90883441</v>
+      </c>
+      <c r="E15" s="4">
+        <v>1.577483444</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="D16" s="4">
+        <v>13.33222645</v>
+      </c>
+      <c r="E16" s="4">
+        <v>1.658940397</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="D17" s="4">
+        <v>14.09117395</v>
+      </c>
+      <c r="E17" s="4">
+        <v>1.698675497</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="D18" s="4">
+        <v>14.75457426</v>
+      </c>
+      <c r="E18" s="4">
+        <v>1.720529801</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="D19" s="4">
+        <v>15.41734803</v>
+      </c>
+      <c r="E19" s="4">
+        <v>1.730463576</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="D20" s="4">
+        <v>16.07980853</v>
+      </c>
+      <c r="E20" s="4">
+        <v>1.734437086</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="D21" s="4">
+        <v>16.74132922</v>
+      </c>
+      <c r="E21" s="4">
+        <v>1.720529801</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="D22" s="4">
+        <v>17.49714403</v>
+      </c>
+      <c r="E22" s="4">
+        <v>1.700662252</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="D23" s="4">
+        <v>18.34673082</v>
+      </c>
+      <c r="E23" s="4">
+        <v>1.664900662</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="D24" s="4">
+        <v>18.91228664</v>
+      </c>
+      <c r="E24" s="4">
+        <v>1.625165563</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="D25" s="4">
+        <v>19.85564543</v>
+      </c>
+      <c r="E25" s="4">
+        <v>1.573509934</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="D26" s="4">
+        <v>20.60989389</v>
+      </c>
+      <c r="E26" s="4">
+        <v>1.52384106</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="D27" s="4">
+        <v>21.26943054</v>
+      </c>
+      <c r="E27" s="4">
+        <v>1.47218543</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="D28" s="4">
+        <v>21.92907162</v>
+      </c>
+      <c r="E28" s="4">
+        <v>1.422516556</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="D29" s="4">
+        <v>22.588295</v>
+      </c>
+      <c r="E29" s="4">
+        <v>1.364900662</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="D30" s="4">
+        <v>23.4374641</v>
+      </c>
+      <c r="E30" s="4">
+        <v>1.321192053</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="D31" s="4">
+        <v>25.04390994</v>
+      </c>
+      <c r="E31" s="4">
+        <v>1.285430464</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="D32" s="4">
+        <v>26.46103659</v>
+      </c>
+      <c r="E32" s="4">
+        <v>1.247682119</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="D33" s="4">
+        <v>28.06675146</v>
+      </c>
+      <c r="E33" s="4">
+        <v>1.198013245</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="D34" s="4">
+        <v>29.10743263</v>
+      </c>
+      <c r="E34" s="4">
+        <v>1.198013245</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="D35" s="4">
+        <v>30.05267104</v>
+      </c>
+      <c r="E35" s="4">
+        <v>1.182119205</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="D36" s="4">
+        <v>32.89151896</v>
+      </c>
+      <c r="E36" s="4">
+        <v>1.194039735</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="D37" s="4">
+        <v>35.06769753</v>
+      </c>
+      <c r="E37" s="4">
+        <v>1.198013245</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="D38" s="4">
+        <v>37.05393038</v>
+      </c>
+      <c r="E38" s="4">
+        <v>1.18807947</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="D39" s="4">
+        <v>39.04152074</v>
+      </c>
+      <c r="E39" s="4">
+        <v>1.20397351</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="D40" s="4">
+        <v>41.02973763</v>
+      </c>
+      <c r="E40" s="4">
+        <v>1.231788079</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="D41" s="4">
+        <v>45.00805103</v>
+      </c>
+      <c r="E41" s="4">
+        <v>1.323178808</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="D42" s="4">
+        <v>46.14260862</v>
+      </c>
+      <c r="E42" s="4">
+        <v>1.309271523</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="D43" s="4">
+        <v>48.0361137</v>
+      </c>
+      <c r="E43" s="4">
+        <v>1.335099338</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="D44" s="4">
+        <v>49.92847014</v>
+      </c>
+      <c r="E44" s="4">
+        <v>1.339072848</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="D45" s="4">
+        <v>52.29271481</v>
+      </c>
+      <c r="E45" s="4">
+        <v>1.321192053</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="D46" s="4">
+        <v>54.75177572</v>
+      </c>
+      <c r="E46" s="4">
+        <v>1.307284768</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="D47" s="4">
+        <v>57.49444991</v>
+      </c>
+      <c r="E47" s="4">
+        <v>1.289403974</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="D48" s="4">
+        <v>60.04717838</v>
+      </c>
+      <c r="E48" s="4">
+        <v>1.257615894</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="D49" s="4">
+        <v>61.65184902</v>
+      </c>
+      <c r="E49" s="4">
+        <v>1.18807947</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="D50" s="4">
+        <v>63.44573442</v>
+      </c>
+      <c r="E50" s="4">
+        <v>1.118543046</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="D51" s="4">
+        <v>65.71182133</v>
+      </c>
+      <c r="E51" s="4">
+        <v>1.033112583</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="D52" s="4">
+        <v>68.54586578</v>
+      </c>
+      <c r="E52" s="4">
+        <v>0.953642384</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="D53" s="4">
+        <v>72.04163978</v>
+      </c>
+      <c r="E53" s="4">
+        <v>0.864238411</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="D54" s="4">
+        <v>74.21332815</v>
+      </c>
+      <c r="E54" s="4">
+        <v>0.782781457</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="D55" s="4">
+        <v>76.76167085</v>
+      </c>
+      <c r="E55" s="4">
+        <v>0.667549669</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="D56" s="4">
+        <v>79.21530175</v>
+      </c>
+      <c r="E56" s="4">
+        <v>0.550331126</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="D57" s="4">
+        <v>80.34735319</v>
+      </c>
+      <c r="E57" s="4">
+        <v>0.488741722</v>
       </c>
     </row>
   </sheetData>
@@ -534,6 +1781,12 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1">
@@ -545,6 +1798,12 @@
       <c r="C2" s="1">
         <v>1.3964</v>
       </c>
+      <c r="D2" s="4">
+        <v>-8.594202298</v>
+      </c>
+      <c r="E2" s="4">
+        <v>-0.76630863</v>
+      </c>
     </row>
     <row r="3">
       <c r="B3" s="3">
@@ -553,13 +1812,113 @@
       <c r="C3" s="1">
         <v>1.4482</v>
       </c>
+      <c r="D3" s="4">
+        <v>-6.197486833</v>
+      </c>
+      <c r="E3" s="4">
+        <v>-0.509572983</v>
+      </c>
     </row>
     <row r="4">
       <c r="B4" s="3">
-        <v>8800000.0</v>
+        <v>9000000.0</v>
       </c>
       <c r="C4" s="1">
         <v>1.4618</v>
+      </c>
+      <c r="D4" s="4">
+        <v>-4.355492888</v>
+      </c>
+      <c r="E4" s="4">
+        <v>-0.300446509</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="D5" s="4">
+        <v>-3.064239207</v>
+      </c>
+      <c r="E5" s="4">
+        <v>-0.16729565</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="D6" s="4">
+        <v>-1.224899432</v>
+      </c>
+      <c r="E6" s="4">
+        <v>0.060741785</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="D7" s="4">
+        <v>0.435283872</v>
+      </c>
+      <c r="E7" s="4">
+        <v>0.231935747</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="D8" s="4">
+        <v>2.09148592</v>
+      </c>
+      <c r="E8" s="4">
+        <v>0.43149615</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="D9" s="4">
+        <v>3.940115291</v>
+      </c>
+      <c r="E9" s="4">
+        <v>0.593345222</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="D10" s="4">
+        <v>5.967901132</v>
+      </c>
+      <c r="E10" s="4">
+        <v>0.812037767</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="D11" s="4">
+        <v>7.625430266</v>
+      </c>
+      <c r="E11" s="4">
+        <v>1.002142689</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="D12" s="4">
+        <v>9.289594824</v>
+      </c>
+      <c r="E12" s="4">
+        <v>1.14497021</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="D13" s="4">
+        <v>10.58217559</v>
+      </c>
+      <c r="E13" s="4">
+        <v>1.268665588</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="D14" s="4">
+        <v>11.17803674</v>
+      </c>
+      <c r="E14" s="4">
+        <v>1.023154868</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="D15" s="4">
+        <v>12.49450504</v>
+      </c>
+      <c r="E15" s="4">
+        <v>0.976651599</v>
       </c>
     </row>
   </sheetData>
@@ -587,6 +1946,12 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2">
@@ -598,6 +1963,12 @@
       <c r="C2" s="1">
         <v>1.2687</v>
       </c>
+      <c r="D2" s="4">
+        <v>-8.594202298</v>
+      </c>
+      <c r="E2" s="4">
+        <v>-0.76630863</v>
+      </c>
     </row>
     <row r="3">
       <c r="B3" s="3">
@@ -606,13 +1977,113 @@
       <c r="C3" s="1">
         <v>1.326</v>
       </c>
+      <c r="D3" s="4">
+        <v>-6.197486833</v>
+      </c>
+      <c r="E3" s="4">
+        <v>-0.509572983</v>
+      </c>
     </row>
     <row r="4">
       <c r="B4" s="3">
-        <v>8800000.0</v>
+        <v>9000000.0</v>
       </c>
       <c r="C4" s="1">
         <v>1.4122</v>
+      </c>
+      <c r="D4" s="4">
+        <v>-4.355492888</v>
+      </c>
+      <c r="E4" s="4">
+        <v>-0.300446509</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="D5" s="4">
+        <v>-3.064239207</v>
+      </c>
+      <c r="E5" s="4">
+        <v>-0.16729565</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="D6" s="4">
+        <v>-1.224899432</v>
+      </c>
+      <c r="E6" s="4">
+        <v>0.060741785</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="D7" s="4">
+        <v>0.435283872</v>
+      </c>
+      <c r="E7" s="4">
+        <v>0.231935747</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="D8" s="4">
+        <v>2.09148592</v>
+      </c>
+      <c r="E8" s="4">
+        <v>0.43149615</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="D9" s="4">
+        <v>3.940115291</v>
+      </c>
+      <c r="E9" s="4">
+        <v>0.593345222</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="D10" s="4">
+        <v>5.967901132</v>
+      </c>
+      <c r="E10" s="4">
+        <v>0.812037767</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="D11" s="4">
+        <v>7.625430266</v>
+      </c>
+      <c r="E11" s="4">
+        <v>1.002142689</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="D12" s="4">
+        <v>9.289594824</v>
+      </c>
+      <c r="E12" s="4">
+        <v>1.14497021</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="D13" s="4">
+        <v>10.58217559</v>
+      </c>
+      <c r="E13" s="4">
+        <v>1.268665588</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="D14" s="4">
+        <v>11.17803674</v>
+      </c>
+      <c r="E14" s="4">
+        <v>1.023154868</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="D15" s="4">
+        <v>12.49450504</v>
+      </c>
+      <c r="E15" s="4">
+        <v>0.976651599</v>
       </c>
     </row>
   </sheetData>

</xml_diff>